<commit_message>
Uploaded Processed Air Temperature Charts - Visor V.0.9.5
</commit_message>
<xml_diff>
--- a/Glaciers_Tables/GUALAS/GUALAS_AIRTEMPERATURE.xlsx
+++ b/Glaciers_Tables/GUALAS/GUALAS_AIRTEMPERATURE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/f_camacho10_uniandes_edu_co/Documents/Copernicus_Master_Olomouc_Documents/Thesis/Github/PatagonianGlaciers/Glaciers_Tables/GUALAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{B307CF71-80B1-4026-BD33-1B50D7F8BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE04BA46-FAC8-4344-8528-D0929F0336DA}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{B307CF71-80B1-4026-BD33-1B50D7F8BADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1DA83C5-D4FA-4B56-A86A-0EC36F1A0796}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -692,7 +692,7 @@
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>GUALES</a:t>
+              <a:t>GUALAS</a:t>
             </a:r>
           </a:p>
           <a:p>

</xml_diff>